<commit_message>
Deploying to gh-pages from @ torstees/ncpi-fhir-ig-2@1b5e4def9df701df38dd4f0fc2bcb151da271852 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-MyPatient.xlsx
+++ b/StructureDefinition-MyPatient.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1754" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1754" uniqueCount="369">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-11-10T21:24:01+00:00</t>
+    <t>2023-11-17T22:43:52+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -87,7 +87,7 @@
     <t>FHIR Version</t>
   </si>
   <si>
-    <t>4.0.1</t>
+    <t>4.3.0</t>
   </si>
   <si>
     <t>Kind</t>
@@ -267,13 +267,16 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}</t>
+dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where(((id.exists() and ('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url)))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(uri) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}</t>
   </si>
   <si>
     <t>Patient[classCode=PAT]</t>
   </si>
   <si>
     <t>ClinicalDocument.recordTarget.patientRole</t>
+  </si>
+  <si>
+    <t>administrative.individual</t>
   </si>
   <si>
     <t>Patient.id</t>
@@ -359,7 +362,7 @@
     <t>preferred</t>
   </si>
   <si>
-    <t>A human language.</t>
+    <t>IETF language tag</t>
   </si>
   <si>
     <t>http://hl7.org/fhir/ValueSet/languages</t>
@@ -417,6 +420,10 @@
     <t>DomainResource.contained</t>
   </si>
   <si>
+    <t xml:space="preserve">dom-r4b:Containing new R4B resources within R4 resources may cause interoperability issues if instances are shared with R4 systems {($this is Citation or $this is Evidence or $this is EvidenceReport or $this is EvidenceVariable or $this is MedicinalProductDefinition or $this is PackagedProductDefinition or $this is AdministrableProductDefinition or $this is Ingredient or $this is ClinicalUseDefinition or $this is RegulatedAuthorization or $this is SubstanceDefinition or $this is SubscriptionStatus or $this is SubscriptionTopic) implies (%resource is Citation or %resource is Evidence or %resource is EvidenceReport or %resource is EvidenceVariable or %resource is MedicinalProductDefinition or %resource is PackagedProductDefinition or %resource is AdministrableProductDefinition or %resource is Ingredient or %resource is ClinicalUseDefinition or %resource is RegulatedAuthorization or %resource is SubstanceDefinition or %resource is SubscriptionStatus or %resource is SubscriptionTopic)}
+</t>
+  </si>
+  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -457,7 +464,7 @@
 Modifier extensions SHALL NOT change the meaning of any elements on Resource or DomainResource (including cannot change the meaning of modifierExtension itself).</t>
   </si>
   <si>
-    <t>Modifier extensions allow for extensions that *cannot* be safely ignored to be clearly distinguished from the vast majority of extensions which can be safely ignored.  This promotes interoperability by eliminating the need for implementers to prohibit the presence of extensions. For further information, see the [definition of modifier extensions](http://hl7.org/fhir/R4/extensibility.html#modifierExtension).</t>
+    <t>Modifier extensions allow for extensions that *cannot* be safely ignored to be clearly distinguished from the vast majority of extensions which can be safely ignored.  This promotes interoperability by eliminating the need for implementers to prohibit the presence of extensions. For further information, see the [definition of modifier extensions](http://hl7.org/fhir/R4B/extensibility.html#modifierExtension).</t>
   </si>
   <si>
     <t>DomainResource.modifierExtension</t>
@@ -602,7 +609,7 @@
     <t>The gender of a person used for administrative purposes.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/administrative-gender|4.0.1</t>
+    <t>http://hl7.org/fhir/ValueSet/administrative-gender|4.3.0</t>
   </si>
   <si>
     <t>player[classCode=PSN|ANM and determinerCode=INSTANCE]/administrativeGender</t>
@@ -804,7 +811,7 @@
     <t>Need to track people you can contact about the patient.</t>
   </si>
   <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+    <t>ele-1:All FHIR elements must have a @value or children unless an empty Parameters resource {hasValue() or (children().count() &gt; id.count()) or $this is Parameters}
 pat-1:SHALL at least contain a contact's details or a reference to an organization {name.exists() or telecom.exists() or address.exists() or organization.exists()}</t>
   </si>
   <si>
@@ -989,6 +996,10 @@
   </si>
   <si>
     <t>If a patient does not speak the local language, interpreters may be required, so languages spoken and proficiency are important things to keep track of both for patient and other persons of interest.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children unless an empty Parameters resource {hasValue() or (children().count() &gt; id.count()) or $this is Parameters}
+</t>
   </si>
   <si>
     <t>LanguageCommunication</t>
@@ -1157,7 +1168,7 @@
     <t>The type of link between this patient resource and another patient resource.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/link-type|4.0.1</t>
+    <t>http://hl7.org/fhir/ValueSet/link-type|4.3.0</t>
   </si>
   <si>
     <t>typeCode</t>
@@ -1752,7 +1763,7 @@
         <v>84</v>
       </c>
       <c r="AM2" t="s" s="2">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="AN2" t="s" s="2">
         <v>78</v>
@@ -1763,10 +1774,10 @@
     </row>
     <row r="3" hidden="true">
       <c r="A3" t="s" s="2">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" t="s" s="2">
@@ -1777,7 +1788,7 @@
         <v>76</v>
       </c>
       <c r="G3" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H3" t="s" s="2">
         <v>78</v>
@@ -1786,19 +1797,19 @@
         <v>78</v>
       </c>
       <c r="J3" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K3" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="L3" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="M3" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="N3" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="O3" s="2"/>
       <c r="P3" t="s" s="2">
@@ -1848,13 +1859,13 @@
         <v>78</v>
       </c>
       <c r="AF3" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AG3" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH3" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AI3" t="s" s="2">
         <v>78</v>
@@ -1880,10 +1891,10 @@
     </row>
     <row r="4" hidden="true">
       <c r="A4" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" t="s" s="2">
@@ -1894,7 +1905,7 @@
         <v>76</v>
       </c>
       <c r="G4" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H4" t="s" s="2">
         <v>78</v>
@@ -1903,16 +1914,16 @@
         <v>78</v>
       </c>
       <c r="J4" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K4" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="L4" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M4" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
@@ -1963,19 +1974,19 @@
         <v>78</v>
       </c>
       <c r="AF4" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AG4" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH4" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AI4" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AJ4" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK4" t="s" s="2">
         <v>78</v>
@@ -1995,10 +2006,10 @@
     </row>
     <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" t="s" s="2">
@@ -2009,28 +2020,28 @@
         <v>76</v>
       </c>
       <c r="G5" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H5" t="s" s="2">
         <v>78</v>
       </c>
       <c r="I5" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J5" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="M5" t="s" s="2">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="N5" t="s" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="O5" s="2"/>
       <c r="P5" t="s" s="2">
@@ -2080,19 +2091,19 @@
         <v>78</v>
       </c>
       <c r="AF5" t="s" s="2">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="AG5" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH5" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AI5" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AJ5" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK5" t="s" s="2">
         <v>78</v>
@@ -2112,10 +2123,10 @@
     </row>
     <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" t="s" s="2">
@@ -2126,7 +2137,7 @@
         <v>76</v>
       </c>
       <c r="G6" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H6" t="s" s="2">
         <v>78</v>
@@ -2138,16 +2149,16 @@
         <v>78</v>
       </c>
       <c r="K6" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="M6" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="N6" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="O6" s="2"/>
       <c r="P6" t="s" s="2">
@@ -2173,13 +2184,13 @@
         <v>78</v>
       </c>
       <c r="X6" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="Y6" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="Z6" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="AA6" t="s" s="2">
         <v>78</v>
@@ -2197,19 +2208,19 @@
         <v>78</v>
       </c>
       <c r="AF6" t="s" s="2">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AG6" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH6" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AI6" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AJ6" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK6" t="s" s="2">
         <v>78</v>
@@ -2229,21 +2240,21 @@
     </row>
     <row r="7" hidden="true">
       <c r="A7" t="s" s="2">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" t="s" s="2">
         <v>76</v>
       </c>
       <c r="G7" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H7" t="s" s="2">
         <v>78</v>
@@ -2255,16 +2266,16 @@
         <v>78</v>
       </c>
       <c r="K7" t="s" s="2">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="L7" t="s" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="M7" t="s" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="N7" t="s" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="O7" s="2"/>
       <c r="P7" t="s" s="2">
@@ -2314,22 +2325,22 @@
         <v>78</v>
       </c>
       <c r="AF7" t="s" s="2">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AG7" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH7" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AI7" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AJ7" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK7" t="s" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="AL7" t="s" s="2">
         <v>78</v>
@@ -2346,14 +2357,14 @@
     </row>
     <row r="8" hidden="true">
       <c r="A8" t="s" s="2">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" t="s" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" t="s" s="2">
@@ -2372,16 +2383,16 @@
         <v>78</v>
       </c>
       <c r="K8" t="s" s="2">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="L8" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="M8" t="s" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="N8" t="s" s="2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="O8" s="2"/>
       <c r="P8" t="s" s="2">
@@ -2431,7 +2442,7 @@
         <v>78</v>
       </c>
       <c r="AF8" t="s" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AG8" t="s" s="2">
         <v>76</v>
@@ -2443,10 +2454,10 @@
         <v>78</v>
       </c>
       <c r="AJ8" t="s" s="2">
-        <v>78</v>
+        <v>130</v>
       </c>
       <c r="AK8" t="s" s="2">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AL8" t="s" s="2">
         <v>78</v>
@@ -2463,14 +2474,14 @@
     </row>
     <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" t="s" s="2">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" t="s" s="2">
@@ -2489,16 +2500,16 @@
         <v>78</v>
       </c>
       <c r="K9" t="s" s="2">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="L9" t="s" s="2">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="M9" t="s" s="2">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="N9" t="s" s="2">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="O9" s="2"/>
       <c r="P9" t="s" s="2">
@@ -2548,7 +2559,7 @@
         <v>78</v>
       </c>
       <c r="AF9" t="s" s="2">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AG9" t="s" s="2">
         <v>76</v>
@@ -2560,10 +2571,10 @@
         <v>78</v>
       </c>
       <c r="AJ9" t="s" s="2">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AK9" t="s" s="2">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AL9" t="s" s="2">
         <v>78</v>
@@ -2580,14 +2591,14 @@
     </row>
     <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" t="s" s="2">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" t="s" s="2">
@@ -2600,25 +2611,25 @@
         <v>78</v>
       </c>
       <c r="I10" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J10" t="s" s="2">
         <v>78</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="M10" t="s" s="2">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="N10" t="s" s="2">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="O10" t="s" s="2">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="P10" t="s" s="2">
         <v>78</v>
@@ -2667,7 +2678,7 @@
         <v>78</v>
       </c>
       <c r="AF10" t="s" s="2">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="AG10" t="s" s="2">
         <v>76</v>
@@ -2679,10 +2690,10 @@
         <v>78</v>
       </c>
       <c r="AJ10" t="s" s="2">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AK10" t="s" s="2">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AL10" t="s" s="2">
         <v>78</v>
@@ -2699,10 +2710,10 @@
     </row>
     <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" t="s" s="2">
@@ -2722,20 +2733,20 @@
         <v>78</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="M11" t="s" s="2">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" t="s" s="2">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="P11" t="s" s="2">
         <v>78</v>
@@ -2784,7 +2795,7 @@
         <v>78</v>
       </c>
       <c r="AF11" t="s" s="2">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="AG11" t="s" s="2">
         <v>76</v>
@@ -2796,19 +2807,19 @@
         <v>78</v>
       </c>
       <c r="AJ11" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK11" t="s" s="2">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="AL11" t="s" s="2">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="AM11" t="s" s="2">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AN11" t="s" s="2">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="AO11" t="s" s="2">
         <v>78</v>
@@ -2816,10 +2827,10 @@
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" t="s" s="2">
@@ -2830,103 +2841,103 @@
         <v>76</v>
       </c>
       <c r="G12" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H12" t="s" s="2">
         <v>78</v>
       </c>
       <c r="I12" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="J12" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="K12" t="s" s="2">
+        <v>155</v>
+      </c>
+      <c r="L12" t="s" s="2">
+        <v>156</v>
+      </c>
+      <c r="M12" t="s" s="2">
+        <v>157</v>
+      </c>
+      <c r="N12" t="s" s="2">
+        <v>158</v>
+      </c>
+      <c r="O12" t="s" s="2">
+        <v>159</v>
+      </c>
+      <c r="P12" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="Q12" t="s" s="2">
+        <v>160</v>
+      </c>
+      <c r="R12" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="S12" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="T12" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="U12" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="V12" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="W12" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="X12" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="Y12" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="Z12" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AA12" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AB12" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AC12" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AD12" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AE12" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AF12" t="s" s="2">
+        <v>154</v>
+      </c>
+      <c r="AG12" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH12" t="s" s="2">
         <v>87</v>
       </c>
-      <c r="J12" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="K12" t="s" s="2">
-        <v>153</v>
-      </c>
-      <c r="L12" t="s" s="2">
-        <v>154</v>
-      </c>
-      <c r="M12" t="s" s="2">
-        <v>155</v>
-      </c>
-      <c r="N12" t="s" s="2">
-        <v>156</v>
-      </c>
-      <c r="O12" t="s" s="2">
-        <v>157</v>
-      </c>
-      <c r="P12" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="Q12" t="s" s="2">
-        <v>158</v>
-      </c>
-      <c r="R12" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="S12" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="T12" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="U12" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="V12" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="W12" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="X12" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="Y12" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="Z12" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AA12" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AB12" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AC12" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AD12" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AE12" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AF12" t="s" s="2">
-        <v>152</v>
-      </c>
-      <c r="AG12" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AH12" t="s" s="2">
-        <v>86</v>
-      </c>
       <c r="AI12" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AJ12" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK12" t="s" s="2">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="AL12" t="s" s="2">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="AM12" t="s" s="2">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="AN12" t="s" s="2">
         <v>78</v>
@@ -2937,10 +2948,10 @@
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" t="s" s="2">
@@ -2948,34 +2959,34 @@
       </c>
       <c r="E13" s="2"/>
       <c r="F13" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G13" t="s" s="2">
         <v>77</v>
       </c>
       <c r="H13" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I13" t="s" s="2">
         <v>78</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="M13" t="s" s="2">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="N13" t="s" s="2">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="O13" t="s" s="2">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="P13" t="s" s="2">
         <v>78</v>
@@ -3024,7 +3035,7 @@
         <v>78</v>
       </c>
       <c r="AF13" t="s" s="2">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="AG13" t="s" s="2">
         <v>76</v>
@@ -3036,19 +3047,19 @@
         <v>78</v>
       </c>
       <c r="AJ13" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK13" t="s" s="2">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="AL13" t="s" s="2">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="AM13" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AN13" t="s" s="2">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="AO13" t="s" s="2">
         <v>78</v>
@@ -3056,10 +3067,10 @@
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" t="s" s="2">
@@ -3079,22 +3090,22 @@
         <v>78</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="N14" t="s" s="2">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="O14" t="s" s="2">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="P14" t="s" s="2">
         <v>78</v>
@@ -3143,7 +3154,7 @@
         <v>78</v>
       </c>
       <c r="AF14" t="s" s="2">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="AG14" t="s" s="2">
         <v>76</v>
@@ -3155,19 +3166,19 @@
         <v>78</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK14" t="s" s="2">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="AL14" t="s" s="2">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="AM14" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AN14" t="s" s="2">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="AO14" t="s" s="2">
         <v>78</v>
@@ -3175,10 +3186,10 @@
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" t="s" s="2">
@@ -3189,7 +3200,7 @@
         <v>76</v>
       </c>
       <c r="G15" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H15" t="s" s="2">
         <v>78</v>
@@ -3198,22 +3209,22 @@
         <v>78</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="M15" t="s" s="2">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="N15" t="s" s="2">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="O15" t="s" s="2">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="P15" t="s" s="2">
         <v>78</v>
@@ -3238,13 +3249,13 @@
         <v>78</v>
       </c>
       <c r="X15" t="s" s="2">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="Y15" t="s" s="2">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="Z15" t="s" s="2">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AA15" t="s" s="2">
         <v>78</v>
@@ -3262,31 +3273,31 @@
         <v>78</v>
       </c>
       <c r="AF15" t="s" s="2">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="AG15" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH15" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AI15" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="AL15" t="s" s="2">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="AM15" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AN15" t="s" s="2">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="AO15" t="s" s="2">
         <v>78</v>
@@ -3294,10 +3305,10 @@
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" t="s" s="2">
@@ -3308,7 +3319,7 @@
         <v>76</v>
       </c>
       <c r="G16" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H16" t="s" s="2">
         <v>78</v>
@@ -3317,22 +3328,22 @@
         <v>78</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="N16" t="s" s="2">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="O16" t="s" s="2">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="P16" t="s" s="2">
         <v>78</v>
@@ -3381,42 +3392,42 @@
         <v>78</v>
       </c>
       <c r="AF16" t="s" s="2">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="AG16" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH16" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AI16" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="AM16" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AN16" t="s" s="2">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="AO16" t="s" s="2">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" t="s" s="2">
@@ -3427,31 +3438,31 @@
         <v>76</v>
       </c>
       <c r="G17" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H17" t="s" s="2">
         <v>78</v>
       </c>
       <c r="I17" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="N17" t="s" s="2">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="O17" t="s" s="2">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="P17" t="s" s="2">
         <v>78</v>
@@ -3500,31 +3511,31 @@
         <v>78</v>
       </c>
       <c r="AF17" t="s" s="2">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="AG17" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH17" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AI17" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="AM17" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AN17" t="s" s="2">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="AO17" t="s" s="2">
         <v>78</v>
@@ -3532,10 +3543,10 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s" s="2">
@@ -3555,22 +3566,22 @@
         <v>78</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="N18" t="s" s="2">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="O18" t="s" s="2">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="P18" t="s" s="2">
         <v>78</v>
@@ -3619,7 +3630,7 @@
         <v>78</v>
       </c>
       <c r="AF18" t="s" s="2">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="AG18" t="s" s="2">
         <v>76</v>
@@ -3631,19 +3642,19 @@
         <v>78</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK18" t="s" s="2">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="AM18" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AN18" t="s" s="2">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="AO18" t="s" s="2">
         <v>78</v>
@@ -3651,10 +3662,10 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s" s="2">
@@ -3665,7 +3676,7 @@
         <v>76</v>
       </c>
       <c r="G19" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H19" t="s" s="2">
         <v>78</v>
@@ -3677,17 +3688,17 @@
         <v>78</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="N19" s="2"/>
       <c r="O19" t="s" s="2">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="P19" t="s" s="2">
         <v>78</v>
@@ -3712,13 +3723,13 @@
         <v>78</v>
       </c>
       <c r="X19" t="s" s="2">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="Y19" t="s" s="2">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="Z19" t="s" s="2">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="AA19" t="s" s="2">
         <v>78</v>
@@ -3736,31 +3747,31 @@
         <v>78</v>
       </c>
       <c r="AF19" t="s" s="2">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="AG19" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH19" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AI19" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="AM19" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AN19" t="s" s="2">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="AO19" t="s" s="2">
         <v>78</v>
@@ -3768,10 +3779,10 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s" s="2">
@@ -3782,7 +3793,7 @@
         <v>76</v>
       </c>
       <c r="G20" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H20" t="s" s="2">
         <v>78</v>
@@ -3794,19 +3805,19 @@
         <v>78</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="N20" t="s" s="2">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="O20" t="s" s="2">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="P20" t="s" s="2">
         <v>78</v>
@@ -3855,31 +3866,31 @@
         <v>78</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="AG20" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH20" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AI20" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="AM20" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AN20" t="s" s="2">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="AO20" t="s" s="2">
         <v>78</v>
@@ -3887,10 +3898,10 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s" s="2">
@@ -3913,19 +3924,19 @@
         <v>78</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="N21" t="s" s="2">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="O21" t="s" s="2">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="P21" t="s" s="2">
         <v>78</v>
@@ -3974,7 +3985,7 @@
         <v>78</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>76</v>
@@ -3986,19 +3997,19 @@
         <v>78</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="AM21" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AN21" t="s" s="2">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="AO21" t="s" s="2">
         <v>78</v>
@@ -4006,10 +4017,10 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
@@ -4032,19 +4043,19 @@
         <v>78</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="N22" t="s" s="2">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="O22" t="s" s="2">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="P22" t="s" s="2">
         <v>78</v>
@@ -4093,7 +4104,7 @@
         <v>78</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>76</v>
@@ -4105,13 +4116,13 @@
         <v>78</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="AM22" t="s" s="2">
         <v>78</v>
@@ -4125,10 +4136,10 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
@@ -4139,7 +4150,7 @@
         <v>76</v>
       </c>
       <c r="G23" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H23" t="s" s="2">
         <v>78</v>
@@ -4151,13 +4162,13 @@
         <v>78</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
@@ -4208,13 +4219,13 @@
         <v>78</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH23" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AI23" t="s" s="2">
         <v>78</v>
@@ -4223,7 +4234,7 @@
         <v>78</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="AL23" t="s" s="2">
         <v>78</v>
@@ -4240,14 +4251,14 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" t="s" s="2">
@@ -4266,16 +4277,16 @@
         <v>78</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="O24" s="2"/>
       <c r="P24" t="s" s="2">
@@ -4325,7 +4336,7 @@
         <v>78</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>76</v>
@@ -4337,10 +4348,10 @@
         <v>78</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="AL24" t="s" s="2">
         <v>78</v>
@@ -4357,14 +4368,14 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" t="s" s="2">
@@ -4377,25 +4388,25 @@
         <v>78</v>
       </c>
       <c r="I25" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="O25" t="s" s="2">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="P25" t="s" s="2">
         <v>78</v>
@@ -4444,7 +4455,7 @@
         <v>78</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>76</v>
@@ -4456,10 +4467,10 @@
         <v>78</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AL25" t="s" s="2">
         <v>78</v>
@@ -4476,10 +4487,10 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s" s="2">
@@ -4502,17 +4513,17 @@
         <v>78</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="N26" s="2"/>
       <c r="O26" t="s" s="2">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="P26" t="s" s="2">
         <v>78</v>
@@ -4537,13 +4548,13 @@
         <v>78</v>
       </c>
       <c r="X26" t="s" s="2">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="Y26" t="s" s="2">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="Z26" t="s" s="2">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="AA26" t="s" s="2">
         <v>78</v>
@@ -4561,7 +4572,7 @@
         <v>78</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>76</v>
@@ -4573,19 +4584,19 @@
         <v>78</v>
       </c>
       <c r="AJ26" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="AM26" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AN26" t="s" s="2">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="AO26" t="s" s="2">
         <v>78</v>
@@ -4593,10 +4604,10 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
@@ -4607,7 +4618,7 @@
         <v>76</v>
       </c>
       <c r="G27" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H27" t="s" s="2">
         <v>78</v>
@@ -4619,17 +4630,17 @@
         <v>78</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="N27" s="2"/>
       <c r="O27" t="s" s="2">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="P27" t="s" s="2">
         <v>78</v>
@@ -4678,31 +4689,31 @@
         <v>78</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH27" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AI27" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AJ27" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="AM27" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AN27" t="s" s="2">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="AO27" t="s" s="2">
         <v>78</v>
@@ -4710,10 +4721,10 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
@@ -4736,19 +4747,19 @@
         <v>78</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="N28" t="s" s="2">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="O28" t="s" s="2">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="P28" t="s" s="2">
         <v>78</v>
@@ -4797,7 +4808,7 @@
         <v>78</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>76</v>
@@ -4809,19 +4820,19 @@
         <v>78</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="AM28" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AN28" t="s" s="2">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="AO28" t="s" s="2">
         <v>78</v>
@@ -4829,10 +4840,10 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
@@ -4843,7 +4854,7 @@
         <v>76</v>
       </c>
       <c r="G29" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H29" t="s" s="2">
         <v>78</v>
@@ -4855,17 +4866,17 @@
         <v>78</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="P29" t="s" s="2">
         <v>78</v>
@@ -4914,31 +4925,31 @@
         <v>78</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH29" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AI29" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AJ29" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="AM29" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AN29" t="s" s="2">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="AO29" t="s" s="2">
         <v>78</v>
@@ -4946,10 +4957,10 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -4960,7 +4971,7 @@
         <v>76</v>
       </c>
       <c r="G30" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H30" t="s" s="2">
         <v>78</v>
@@ -4972,17 +4983,17 @@
         <v>78</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="P30" t="s" s="2">
         <v>78</v>
@@ -5007,13 +5018,13 @@
         <v>78</v>
       </c>
       <c r="X30" t="s" s="2">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="Y30" t="s" s="2">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="Z30" t="s" s="2">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AA30" t="s" s="2">
         <v>78</v>
@@ -5031,31 +5042,31 @@
         <v>78</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH30" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AI30" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="AM30" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AN30" t="s" s="2">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="AO30" t="s" s="2">
         <v>78</v>
@@ -5063,10 +5074,10 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -5077,7 +5088,7 @@
         <v>76</v>
       </c>
       <c r="G31" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H31" t="s" s="2">
         <v>78</v>
@@ -5089,17 +5100,17 @@
         <v>78</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="P31" t="s" s="2">
         <v>78</v>
@@ -5148,31 +5159,31 @@
         <v>78</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH31" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AI31" t="s" s="2">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="AM31" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AN31" t="s" s="2">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="AO31" t="s" s="2">
         <v>78</v>
@@ -5180,10 +5191,10 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -5194,7 +5205,7 @@
         <v>76</v>
       </c>
       <c r="G32" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H32" t="s" s="2">
         <v>78</v>
@@ -5206,13 +5217,13 @@
         <v>78</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
@@ -5263,25 +5274,25 @@
         <v>78</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH32" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AI32" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="AM32" t="s" s="2">
         <v>78</v>
@@ -5295,10 +5306,10 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -5321,19 +5332,19 @@
         <v>78</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="N33" t="s" s="2">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="O33" t="s" s="2">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="P33" t="s" s="2">
         <v>78</v>
@@ -5382,7 +5393,7 @@
         <v>78</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>76</v>
@@ -5394,13 +5405,13 @@
         <v>78</v>
       </c>
       <c r="AJ33" t="s" s="2">
-        <v>98</v>
+        <v>313</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="AM33" t="s" s="2">
         <v>78</v>
@@ -5414,10 +5425,10 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -5428,7 +5439,7 @@
         <v>76</v>
       </c>
       <c r="G34" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H34" t="s" s="2">
         <v>78</v>
@@ -5440,13 +5451,13 @@
         <v>78</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
@@ -5497,13 +5508,13 @@
         <v>78</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH34" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AI34" t="s" s="2">
         <v>78</v>
@@ -5512,7 +5523,7 @@
         <v>78</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="AL34" t="s" s="2">
         <v>78</v>
@@ -5529,14 +5540,14 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" t="s" s="2">
@@ -5555,16 +5566,16 @@
         <v>78</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="N35" t="s" s="2">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="O35" s="2"/>
       <c r="P35" t="s" s="2">
@@ -5614,7 +5625,7 @@
         <v>78</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>76</v>
@@ -5626,10 +5637,10 @@
         <v>78</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="AL35" t="s" s="2">
         <v>78</v>
@@ -5646,14 +5657,14 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" t="s" s="2">
@@ -5666,25 +5677,25 @@
         <v>78</v>
       </c>
       <c r="I36" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="N36" t="s" s="2">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="O36" t="s" s="2">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="P36" t="s" s="2">
         <v>78</v>
@@ -5733,7 +5744,7 @@
         <v>78</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>76</v>
@@ -5745,10 +5756,10 @@
         <v>78</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AL36" t="s" s="2">
         <v>78</v>
@@ -5765,10 +5776,10 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -5776,10 +5787,10 @@
       </c>
       <c r="E37" s="2"/>
       <c r="F37" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G37" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H37" t="s" s="2">
         <v>78</v>
@@ -5791,19 +5802,19 @@
         <v>78</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="N37" t="s" s="2">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="O37" t="s" s="2">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="P37" t="s" s="2">
         <v>78</v>
@@ -5828,13 +5839,13 @@
         <v>78</v>
       </c>
       <c r="X37" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="Y37" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="Z37" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="AA37" t="s" s="2">
         <v>78</v>
@@ -5852,31 +5863,31 @@
         <v>78</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="AG37" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AH37" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AI37" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="AM37" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AN37" t="s" s="2">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="AO37" t="s" s="2">
         <v>78</v>
@@ -5884,10 +5895,10 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
@@ -5898,7 +5909,7 @@
         <v>76</v>
       </c>
       <c r="G38" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H38" t="s" s="2">
         <v>78</v>
@@ -5910,19 +5921,19 @@
         <v>78</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="N38" t="s" s="2">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="O38" t="s" s="2">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="P38" t="s" s="2">
         <v>78</v>
@@ -5971,31 +5982,31 @@
         <v>78</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH38" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AI38" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="AM38" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AN38" t="s" s="2">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="AO38" t="s" s="2">
         <v>78</v>
@@ -6003,14 +6014,14 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" t="s" s="2">
@@ -6029,16 +6040,16 @@
         <v>78</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="N39" t="s" s="2">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="O39" s="2"/>
       <c r="P39" t="s" s="2">
@@ -6088,7 +6099,7 @@
         <v>78</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>76</v>
@@ -6100,19 +6111,19 @@
         <v>78</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="AM39" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AN39" t="s" s="2">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="AO39" t="s" s="2">
         <v>78</v>
@@ -6120,10 +6131,10 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -6134,7 +6145,7 @@
         <v>76</v>
       </c>
       <c r="G40" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H40" t="s" s="2">
         <v>78</v>
@@ -6143,22 +6154,22 @@
         <v>78</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="O40" t="s" s="2">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="P40" t="s" s="2">
         <v>78</v>
@@ -6207,25 +6218,25 @@
         <v>78</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH40" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AI40" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="AM40" t="s" s="2">
         <v>78</v>
@@ -6239,10 +6250,10 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
@@ -6259,25 +6270,25 @@
         <v>78</v>
       </c>
       <c r="I41" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="N41" t="s" s="2">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="O41" t="s" s="2">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="P41" t="s" s="2">
         <v>78</v>
@@ -6326,7 +6337,7 @@
         <v>78</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>76</v>
@@ -6338,13 +6349,13 @@
         <v>78</v>
       </c>
       <c r="AJ41" t="s" s="2">
-        <v>98</v>
+        <v>313</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="AM41" t="s" s="2">
         <v>78</v>
@@ -6358,10 +6369,10 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -6372,7 +6383,7 @@
         <v>76</v>
       </c>
       <c r="G42" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H42" t="s" s="2">
         <v>78</v>
@@ -6384,13 +6395,13 @@
         <v>78</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" s="2"/>
@@ -6441,13 +6452,13 @@
         <v>78</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH42" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AI42" t="s" s="2">
         <v>78</v>
@@ -6456,7 +6467,7 @@
         <v>78</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="AL42" t="s" s="2">
         <v>78</v>
@@ -6473,14 +6484,14 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" t="s" s="2">
@@ -6499,16 +6510,16 @@
         <v>78</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="N43" t="s" s="2">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="O43" s="2"/>
       <c r="P43" t="s" s="2">
@@ -6558,7 +6569,7 @@
         <v>78</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>76</v>
@@ -6570,10 +6581,10 @@
         <v>78</v>
       </c>
       <c r="AJ43" t="s" s="2">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="AL43" t="s" s="2">
         <v>78</v>
@@ -6590,14 +6601,14 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" t="s" s="2">
@@ -6610,25 +6621,25 @@
         <v>78</v>
       </c>
       <c r="I44" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="N44" t="s" s="2">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="O44" t="s" s="2">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="P44" t="s" s="2">
         <v>78</v>
@@ -6677,7 +6688,7 @@
         <v>78</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>76</v>
@@ -6689,10 +6700,10 @@
         <v>78</v>
       </c>
       <c r="AJ44" t="s" s="2">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AL44" t="s" s="2">
         <v>78</v>
@@ -6709,10 +6720,10 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -6720,10 +6731,10 @@
       </c>
       <c r="E45" s="2"/>
       <c r="F45" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G45" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H45" t="s" s="2">
         <v>78</v>
@@ -6732,19 +6743,19 @@
         <v>78</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="N45" t="s" s="2">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="O45" s="2"/>
       <c r="P45" t="s" s="2">
@@ -6794,31 +6805,31 @@
         <v>78</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="AG45" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AH45" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AI45" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AJ45" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK45" t="s" s="2">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="AM45" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AN45" t="s" s="2">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="AO45" t="s" s="2">
         <v>78</v>
@@ -6826,10 +6837,10 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
@@ -6837,10 +6848,10 @@
       </c>
       <c r="E46" s="2"/>
       <c r="F46" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G46" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H46" t="s" s="2">
         <v>78</v>
@@ -6849,16 +6860,16 @@
         <v>78</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" s="2"/>
@@ -6885,49 +6896,49 @@
         <v>78</v>
       </c>
       <c r="X46" t="s" s="2">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="Y46" t="s" s="2">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="Z46" t="s" s="2">
+        <v>367</v>
+      </c>
+      <c r="AA46" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AB46" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AC46" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AD46" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AE46" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AF46" t="s" s="2">
         <v>364</v>
       </c>
-      <c r="AA46" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AB46" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AC46" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AD46" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AE46" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AF46" t="s" s="2">
-        <v>361</v>
-      </c>
       <c r="AG46" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AH46" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AI46" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AJ46" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK46" t="s" s="2">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="AM46" t="s" s="2">
         <v>78</v>

</xml_diff>